<commit_message>
Display the contents of an excel sheet on the web page.
</commit_message>
<xml_diff>
--- a/App_Data/uploads/Test1.xlsx
+++ b/App_Data/uploads/Test1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,33 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>Some name.</t>
+  </si>
+  <si>
+    <t>ItemPrice</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,17 +65,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +376,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Load Excel data into the database.
</commit_message>
<xml_diff>
--- a/App_Data/uploads/Test1.xlsx
+++ b/App_Data/uploads/Test1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
   <si>
     <t>ItemName</t>
   </si>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +437,118 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add three types of LinqToExcel queries.
</commit_message>
<xml_diff>
--- a/App_Data/uploads/Test1.xlsx
+++ b/App_Data/uploads/Test1.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sale Items" sheetId="2" r:id="rId2"/>
+    <sheet name="Wierd Columns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>ItemName</t>
   </si>
@@ -23,6 +25,18 @@
   </si>
   <si>
     <t>ItemPrice</t>
+  </si>
+  <si>
+    <t>Some sale item</t>
+  </si>
+  <si>
+    <t>The Prices We Charge</t>
+  </si>
+  <si>
+    <t>What We Call Our Items</t>
+  </si>
+  <si>
+    <t>Superstar Squash</t>
   </si>
 </sst>
 </file>
@@ -377,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -418,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -426,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,7 +448,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -442,7 +456,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -458,95 +472,145 @@
         <v>1</v>
       </c>
       <c r="B9" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
         <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add code to read and render the worksheet and column names from an excel file with linq to excel.
</commit_message>
<xml_diff>
--- a/App_Data/uploads/Test1.xlsx
+++ b/App_Data/uploads/Test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,18 +474,6 @@
       <c r="B9" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>